<commit_message>
feat: add new data
</commit_message>
<xml_diff>
--- a/2. Questions/Questions and Answers.xlsx
+++ b/2. Questions/Questions and Answers.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Desktop\NLP_Student_Manual_Chatbot\2. Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC1D455-6437-425B-BBF0-5B74C807598F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA3EA6-F09F-4FBC-BF9B-0A97A5295B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{40531BC3-4381-4E9F-9043-CEEA158DC373}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
     <sheet name="Sections" sheetId="2" r:id="rId2"/>
-    <sheet name="Articles" sheetId="4" r:id="rId3"/>
+    <sheet name="Abbreviations" sheetId="5" r:id="rId3"/>
+    <sheet name="Articles" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="265">
   <si>
     <t>QUESTION</t>
   </si>
@@ -112,9 +113,6 @@
     <t>TOPIC</t>
   </si>
   <si>
-    <t>What is the full name of USC?</t>
-  </si>
-  <si>
     <t>University of San Carlos</t>
   </si>
   <si>
@@ -266,13 +264,594 @@
   </si>
   <si>
     <t>Additional Enrollment Steps (Scholarship and Financial Assistance)</t>
+  </si>
+  <si>
+    <t>Society of the Divine Word (SVD) missionaries</t>
+  </si>
+  <si>
+    <t>How many campuses does the university have?</t>
+  </si>
+  <si>
+    <t>North Campus, South Campus, Talamban Campus, Downtown Campus, Montessori Campus</t>
+  </si>
+  <si>
+    <t>ABBREVIATION</t>
+  </si>
+  <si>
+    <t>MEANING</t>
+  </si>
+  <si>
+    <t>USC</t>
+  </si>
+  <si>
+    <t>SVD</t>
+  </si>
+  <si>
+    <t>Society of the Divine Word</t>
+  </si>
+  <si>
+    <t>PAASCU</t>
+  </si>
+  <si>
+    <t>Philippine Accrediting Association of Schools, Colleges, and Universities</t>
+  </si>
+  <si>
+    <t>PTC-ACBET</t>
+  </si>
+  <si>
+    <t>Philippine Technological Council-Accreditation and Certification Board for Engineering and Technology</t>
+  </si>
+  <si>
+    <t>CHED</t>
+  </si>
+  <si>
+    <t>Commission on Higher Education</t>
+  </si>
+  <si>
+    <t>COE</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>Center of Excellence</t>
+  </si>
+  <si>
+    <t>Center of Development</t>
+  </si>
+  <si>
+    <t>How many engineering programs are accredited by the Philippine Technological Council-Accreditation and Certification Board for Engineering and Technology?</t>
+  </si>
+  <si>
+    <t>How many Centers of Excellence did the Commission on Higher Education grant to USC?</t>
+  </si>
+  <si>
+    <t>451 to 500 in QS University Rankings for Asia 2021 and 7 among the 100 best universities in the Philippines in 2023 per EduRank</t>
+  </si>
+  <si>
+    <t>What is the ranking of University of San Carlos?</t>
+  </si>
+  <si>
+    <t>What is the university's ranking based on?</t>
+  </si>
+  <si>
+    <t>research outputs, non-academic prominence, non
+academic performance and alumni influence</t>
+  </si>
+  <si>
+    <t>How much external research grants has the university drawn?</t>
+  </si>
+  <si>
+    <t>What are the campuses of the university?</t>
+  </si>
+  <si>
+    <t>PHP298M (~USD5.68M) between AY 2018-2021</t>
+  </si>
+  <si>
+    <t>How many secondary journals did the university publish?</t>
+  </si>
+  <si>
+    <t>What are the secondary journals published by the university?</t>
+  </si>
+  <si>
+    <t>The Philippine Scientist, the Philippine Quarterly of Culture and Society, and Devotio: Journal of Business and Economic Studies</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>Eight</t>
+  </si>
+  <si>
+    <t>Twelve</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>How are additional support for researchers available?</t>
+  </si>
+  <si>
+    <t>through offices or committees providing ethics review, intellectual property and innovation and technology support, and animal care and use</t>
+  </si>
+  <si>
+    <t>What journals does the University's library system subscribe to?</t>
+  </si>
+  <si>
+    <t>Web of Science and Science Direct</t>
+  </si>
+  <si>
+    <t>How many patents have been filed by the university?</t>
+  </si>
+  <si>
+    <t>Nineteen</t>
+  </si>
+  <si>
+    <t>How many undergraduate and graduate scholars does the university have at any given time?</t>
+  </si>
+  <si>
+    <t>More than 600</t>
+  </si>
+  <si>
+    <t>The university has been designated as a Donee Institution since when?</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>When did the University of San Carlos become a university?</t>
+  </si>
+  <si>
+    <t>Who first administered the university?</t>
+  </si>
+  <si>
+    <t>When was the university first administered?</t>
+  </si>
+  <si>
+    <t>1935</t>
+  </si>
+  <si>
+    <t>QS</t>
+  </si>
+  <si>
+    <t>Quacquarelli Symonds</t>
+  </si>
+  <si>
+    <t>What are the two statements that the university's catholic identity is embodied in?</t>
+  </si>
+  <si>
+    <t>Education with a Mission and Witness to the Word</t>
+  </si>
+  <si>
+    <t>What is the vision of the university?</t>
+  </si>
+  <si>
+    <t>What is the mission of the university?</t>
+  </si>
+  <si>
+    <t>What are the core values of the university?</t>
+  </si>
+  <si>
+    <t>The University of San Carlos sees:
+ • a WORLD where the darkness of sin and the night of unbelief vanish 
+before the light of the Word and the Spirit of grace
+ • a SOCIETY where citizens are competent, noble in character, and 
+community-oriented
+ • what they know, they apply justly and honestly;
+ • what they do not know, they seek to learn;
+ • what they do not have, they endeavor to acquire;
+ • what they have, they share</t>
+  </si>
+  <si>
+    <t>What does scientia mean?</t>
+  </si>
+  <si>
+    <t>professionally competent and skilled</t>
+  </si>
+  <si>
+    <t>What does virtus mean?</t>
+  </si>
+  <si>
+    <t>noble character and are value-driven</t>
+  </si>
+  <si>
+    <t>What does devotio mean?</t>
+  </si>
+  <si>
+    <t>dedicated to social transformation</t>
+  </si>
+  <si>
+    <t>Integrity; Excellence; Commitment; Social responsibility; Evangelization; and Leadership</t>
+  </si>
+  <si>
+    <t>The University of San Carlos is a Catholic institution of learning that embodies the principles of academic discipline of San Carlos Borromeo and the missionary charism of the Society of the Divine Word (SVD). 
+It aims to develop competent and socially responsible professionals and lifelong learners in an environment that fosters excellence in the academic core processes of teaching-learning, research, and community extension service. 
+Its mission is to provide timely, relevant, and transformative academic programs responsive to the needs of the local, national, and global communities in a rapidly changing world.</t>
+  </si>
+  <si>
+    <t>What does integrity mean?</t>
+  </si>
+  <si>
+    <t>Carolinians shall reflect in their personal and professional life the ideals of the Catholic university as “an academic community, which, in a rigorous and critical fashion, assists in the protection and advancement of human dignity and of a cultural heritage through research, teaching and extension services to the local, national and international communities”</t>
+  </si>
+  <si>
+    <t>What does excellence mean?</t>
+  </si>
+  <si>
+    <t>Carolinians shall constantly strive to attain the highest standards in their respective fields.</t>
+  </si>
+  <si>
+    <t>What does commitment mean?</t>
+  </si>
+  <si>
+    <t>Carolinians shall bear in mind that the ultimate goal of the University is the transformation of communities, especially in the Visayas and Mindanao, through the provision of quality basic and higher education.</t>
+  </si>
+  <si>
+    <t>What does social responsibility mean?</t>
+  </si>
+  <si>
+    <t>Carolinians shall strive to provide themselves and the students an understanding of and effective tools for addressing the prevailing social realities in the country. As far as possible, they shall volunteer their expertise and contribute to effective social and civic programs in the local community, through initiatives organized by themselves, their respective departments and relevant external organizations.</t>
+  </si>
+  <si>
+    <t>What does evangelization mean?</t>
+  </si>
+  <si>
+    <t>Carolinians shall seek to understand the values and mores of local cultures and enrich them through gospel values and the teachings of the Church. In a privileged manner, they shall, in solidarity with the Philippines Southern Province of the Society of Divine Word, support the missionary apostolate in the Visayas and Mindanao.</t>
+  </si>
+  <si>
+    <t>What does leadership mean?</t>
+  </si>
+  <si>
+    <t>Carolinians, not only in positions of authority but also in their own personal capacity, shall strive to set the conditions for reflection and learning on their respective educational tasks, both in their departments and in the local community, foster norms of behavior befitting a Witness to the Word and exhibit these norms in their own way of life.</t>
+  </si>
+  <si>
+    <t>What does the university seal depict?</t>
+  </si>
+  <si>
+    <t>a shield on either side by seven laurel leaves</t>
+  </si>
+  <si>
+    <t>What do the laurel leaves stand for?</t>
+  </si>
+  <si>
+    <t>wisdom, understanding, counsel, fortitude, knowledge, piety, and fear of the Lord</t>
+  </si>
+  <si>
+    <t>What do the three parts of the shield symbolize?</t>
+  </si>
+  <si>
+    <t>SVD, Cebu City, and knowledge, education, and the Word of God.</t>
+  </si>
+  <si>
+    <t>What do the three stars in the university seal represent?</t>
+  </si>
+  <si>
+    <t>The three major island groups of the Philippines: Luzon, Visayas, and Mindanao</t>
+  </si>
+  <si>
+    <t>Where is the university historically linked to?</t>
+  </si>
+  <si>
+    <t>a small colegio established in honor of San Ildefonso by the Jesuit priests Antonio Sedeño, Alonso de Humanes, Mateo Sanchez, and a lay brother Gaspar Garay on 21 August 1595</t>
+  </si>
+  <si>
+    <t>When was the university granted university status by the government?</t>
+  </si>
+  <si>
+    <t>1 July 1948</t>
+  </si>
+  <si>
+    <t>When did the university conferred the Bachelor's degree to its first graduates?</t>
+  </si>
+  <si>
+    <t>1894</t>
+  </si>
+  <si>
+    <t>When did the university transfer to its present site?</t>
+  </si>
+  <si>
+    <t>1930</t>
+  </si>
+  <si>
+    <t>In 1935, the Colegio de San Carlos was placed under what religious order?</t>
+  </si>
+  <si>
+    <t>Societas Verbi Divini (SVD)</t>
+  </si>
+  <si>
+    <t>When was the college of pharmacy added?</t>
+  </si>
+  <si>
+    <t>1947</t>
+  </si>
+  <si>
+    <t>When was the university North Campus opened?</t>
+  </si>
+  <si>
+    <t>1956</t>
+  </si>
+  <si>
+    <t>When was the university South Campus opened?</t>
+  </si>
+  <si>
+    <t>1962</t>
+  </si>
+  <si>
+    <t>Where is the university North Campus located?</t>
+  </si>
+  <si>
+    <t>along Gen. Maxilom Avenue</t>
+  </si>
+  <si>
+    <t>J. Alcantara Street</t>
+  </si>
+  <si>
+    <t>Where is the university South Campus located?</t>
+  </si>
+  <si>
+    <t>When was the university Talamban Campus opened?</t>
+  </si>
+  <si>
+    <t>1963</t>
+  </si>
+  <si>
+    <t>The university Talamban Campus became known as what by 1965?</t>
+  </si>
+  <si>
+    <t>By what year was the university Talamban Campus known as the Technological center?</t>
+  </si>
+  <si>
+    <t>1965</t>
+  </si>
+  <si>
+    <t>Technological center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When was the Josef Baumgartner Learning Resource Center built? </t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>When was the Arts and Sciences Building built?</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>When was the Science Building built?</t>
+  </si>
+  <si>
+    <t>1981</t>
+  </si>
+  <si>
+    <t>When were the Talamban Campus Dormitories built?</t>
+  </si>
+  <si>
+    <t>What was the Arts and Sciences building later named to?</t>
+  </si>
+  <si>
+    <t>Philip van Engelen Building</t>
+  </si>
+  <si>
+    <t>1938</t>
+  </si>
+  <si>
+    <t>When was the college of Engineering added?</t>
+  </si>
+  <si>
+    <t>When was the college of Education added?</t>
+  </si>
+  <si>
+    <t>1939</t>
+  </si>
+  <si>
+    <t>When was the Michael Richartz building built?</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>What was the Engineering Conference center renamed to?</t>
+  </si>
+  <si>
+    <t>Michael Richartz Building</t>
+  </si>
+  <si>
+    <t>What was the old name of Michael Richartz Building ?</t>
+  </si>
+  <si>
+    <t>Engineering Conference Center</t>
+  </si>
+  <si>
+    <t>In what year did The Arts Division of the College of Arts and Sciences transferred to Talamban Campus?</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>When was the Language Academy built?</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>Since when did the Comission of Higher Education award full autonomy status to the university?</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>What award did the university's Cebuano Studies Center receive in 2009?</t>
+  </si>
+  <si>
+    <t>Region VII Winner for CHED Best Higher Education Research Program</t>
+  </si>
+  <si>
+    <t>What are the three university saints?</t>
+  </si>
+  <si>
+    <t>San Carlos Borromeo (1538-1584), St. Arnold Janssen (1837-1909), St. Joseph Freinademetz (1852-1908)</t>
+  </si>
+  <si>
+    <t>When is the feast day of St. Charles Borromeo?</t>
+  </si>
+  <si>
+    <t>November 4</t>
+  </si>
+  <si>
+    <t>Who is the founder of the Society of the Divine Word?</t>
+  </si>
+  <si>
+    <t>St. Arnold Janssen</t>
+  </si>
+  <si>
+    <t>What society manages the university?</t>
+  </si>
+  <si>
+    <t>What are the 4 zones of the SVD missionary world?</t>
+  </si>
+  <si>
+    <t>Asia-Pacific (ASPAC), Africa-Madagascar (AFRAM), America (PANAM) and Europe (EUROPA)</t>
+  </si>
+  <si>
+    <t>What are the vice presidents assisting the university president?</t>
+  </si>
+  <si>
+    <t>How many vice presidents are assisting the university president?</t>
+  </si>
+  <si>
+    <t>Vice President for Academic Affairs, Vice President for Administration, Vice President for Finance</t>
+  </si>
+  <si>
+    <t>How many members are in the Board of Trustees of the university?</t>
+  </si>
+  <si>
+    <t>Ten</t>
+  </si>
+  <si>
+    <t>What are the offices attached to the office of the president?</t>
+  </si>
+  <si>
+    <t>the University Chaplain, the Legal Counsel, the Institutional Planning and Quality Assurance (IPQA), the Knowledge, Technology and Transfer Office (KTTO), the Corporate Communications Office, the Office of the Presidential Assistant for Mission and Spirituality (PAMS), and Internal Audit Office</t>
+  </si>
+  <si>
+    <t>What are the offices headed by the Vice President for Academic Affairs?</t>
+  </si>
+  <si>
+    <t>University Academic Council and its Committees, Deans and Chairs, Office of the University Registrar, Research, Development, Extension and Publications Office (RDEPO), External Relations and Internationalization Office (ERIO), Community Extension Services (CES), Library System, National Service Training Program (NSTP), USC Publishing House.</t>
+  </si>
+  <si>
+    <t>What are the offices headed by the Vice President for Administration?</t>
+  </si>
+  <si>
+    <t>Advancement Office, Information Resources Management Office (IRMO), Student Affairs and Services Office (SASO), Office of Administrator of Properties (OAP), Data Privacy Office (DPO), Office of Security and Safety, and Human Resource Management Office (HRMO).</t>
+  </si>
+  <si>
+    <t>IPQA</t>
+  </si>
+  <si>
+    <t>Institutional Planning and Quality Assurance</t>
+  </si>
+  <si>
+    <t>PAMS</t>
+  </si>
+  <si>
+    <t>Internal Audit Office</t>
+  </si>
+  <si>
+    <t>OVPAA</t>
+  </si>
+  <si>
+    <t>Office of the Vice President for Academic Affairs</t>
+  </si>
+  <si>
+    <t>RDEPO</t>
+  </si>
+  <si>
+    <t>Research, Development, Extension and Publications Office</t>
+  </si>
+  <si>
+    <t>ERIO</t>
+  </si>
+  <si>
+    <t>External Relations and Internationalization Office</t>
+  </si>
+  <si>
+    <t>Community Extension Services</t>
+  </si>
+  <si>
+    <t>CES</t>
+  </si>
+  <si>
+    <t>National Service Training Program</t>
+  </si>
+  <si>
+    <t>NSTP</t>
+  </si>
+  <si>
+    <t>VPAd</t>
+  </si>
+  <si>
+    <t>Vice President for Administration</t>
+  </si>
+  <si>
+    <t>IRMO</t>
+  </si>
+  <si>
+    <t>Information Resources Management Office</t>
+  </si>
+  <si>
+    <t>Student Affairs and Services Office</t>
+  </si>
+  <si>
+    <t>SASO</t>
+  </si>
+  <si>
+    <t>Office of Administrator of Properties</t>
+  </si>
+  <si>
+    <t>OAP</t>
+  </si>
+  <si>
+    <t>DPO</t>
+  </si>
+  <si>
+    <t>HRMO</t>
+  </si>
+  <si>
+    <t>Data Privacy Office</t>
+  </si>
+  <si>
+    <t>Human Resource Management Office</t>
+  </si>
+  <si>
+    <t>OAASJ</t>
+  </si>
+  <si>
+    <t>Office of Alumni Affairs, Scholarship and Job Placement Office</t>
+  </si>
+  <si>
+    <t>Office of Naming Rights, Endowments and Scholarships</t>
+  </si>
+  <si>
+    <t>ONES</t>
+  </si>
+  <si>
+    <t>OSFA</t>
+  </si>
+  <si>
+    <t>Office of Student Formation and Activities</t>
+  </si>
+  <si>
+    <t>CDC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +866,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -309,7 +894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -317,6 +902,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,17 +1261,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB12015F-344C-4C50-9691-EBF7D05F5397}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="73.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="49" style="5" customWidth="1"/>
+    <col min="3" max="3" width="60" style="5" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
@@ -670,27 +1279,788 @@
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>25</v>
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>2</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>2</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="201.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>2</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>2</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>2</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>2</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>2</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>2</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>2</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>2</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>3</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>3</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>3</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>4</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>4</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>4</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>4</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>4</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>4</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>4</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>4</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>4</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>4</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>4</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>4</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>4</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>4</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>4</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="3">
+        <v>4</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="3">
+        <v>4</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C53" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="3">
+        <v>4</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="3">
+        <v>4</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="3">
+        <v>4</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="3">
+        <v>4</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="3">
+        <v>4</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="3">
+        <v>4</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="3">
+        <v>4</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="3">
+        <v>4</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="3">
+        <v>4</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="3">
+        <v>5</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="3">
+        <v>5</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="3">
+        <v>5</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="3">
+        <v>5</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="3">
+        <v>5</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C67" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="3">
+        <v>6</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B69" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B70" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B71" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B72" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B73" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -702,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CFA4CAE-A54D-4C8C-9F41-F390D4C38DA7}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D30" sqref="A29:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -750,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -764,7 +2134,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -778,7 +2148,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -792,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -806,7 +2176,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -820,7 +2190,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -834,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -848,7 +2218,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -862,7 +2232,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -876,7 +2246,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -890,7 +2260,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -904,7 +2274,7 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -918,7 +2288,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -932,7 +2302,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -946,7 +2316,7 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -960,7 +2330,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -974,7 +2344,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -988,7 +2358,7 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1002,7 +2372,7 @@
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1016,7 +2386,7 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1030,7 +2400,7 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1044,7 +2414,7 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1058,7 +2428,7 @@
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1072,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1086,7 +2456,7 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1100,7 +2470,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1114,7 +2484,7 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1128,7 +2498,7 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1142,7 +2512,7 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1156,7 +2526,7 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1170,7 +2540,7 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1184,7 +2554,7 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1198,7 +2568,7 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1212,7 +2582,7 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1226,7 +2596,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1240,7 +2610,7 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1492,7 +2862,7 @@
         <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1506,7 +2876,7 @@
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1530,11 +2900,235 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A0C351-3687-474E-A31D-3B46FA24EFD7}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="82.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>248</v>
+      </c>
+      <c r="B18" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>254</v>
+      </c>
+      <c r="B21" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>255</v>
+      </c>
+      <c r="B22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>258</v>
+      </c>
+      <c r="B23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>261</v>
+      </c>
+      <c r="B24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>262</v>
+      </c>
+      <c r="B25" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9944EF6B-5BE4-474D-89C0-C1D33ABC3D1D}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1544,10 +3138,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1555,7 +3149,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1563,7 +3157,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1571,7 +3165,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1579,7 +3173,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1587,7 +3181,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1595,7 +3189,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1603,7 +3197,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1611,7 +3205,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1619,7 +3213,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1627,7 +3221,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add abbreviations and divided article 60 and 61
</commit_message>
<xml_diff>
--- a/2. Questions/Questions and Answers.xlsx
+++ b/2. Questions/Questions and Answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marc\Desktop\NLP_Student_Manual_Chatbot\2. Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C326AA0D-B9E8-4D31-A2B4-DEB8C682EEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90C683D-91B4-4322-A9ED-9922ECDFD72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="3" activeTab="3" xr2:uid="{40531BC3-4381-4E9F-9043-CEEA158DC373}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{40531BC3-4381-4E9F-9043-CEEA158DC373}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="697">
   <si>
     <t>QUESTION</t>
   </si>
@@ -777,12 +777,6 @@
   </si>
   <si>
     <t>Human Resource Management Office</t>
-  </si>
-  <si>
-    <t>OAASJ</t>
-  </si>
-  <si>
-    <t>Office of Alumni Affairs, Scholarship and Job Placement Office</t>
   </si>
   <si>
     <t>Office of Naming Rights, Endowments and Scholarships</t>
@@ -2162,9 +2156,6 @@
   </si>
   <si>
     <t>CHL Rationale and Aims</t>
-  </si>
-  <si>
-    <t>Office of Alumni Affairs, Scholarships and Job Placement</t>
   </si>
   <si>
     <t>OAASJP</t>
@@ -2286,7 +2277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2320,8 +2311,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2887,7 +2876,7 @@
         <v>114</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="201.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3478,10 +3467,10 @@
         <v>6</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3489,10 +3478,10 @@
         <v>6</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -3500,10 +3489,10 @@
         <v>6</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3511,10 +3500,10 @@
         <v>6</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -3522,10 +3511,10 @@
         <v>6</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -3533,10 +3522,10 @@
         <v>6</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3544,10 +3533,10 @@
         <v>6</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -3555,10 +3544,10 @@
         <v>6</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -3566,10 +3555,10 @@
         <v>6</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3577,10 +3566,10 @@
         <v>7</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -3588,10 +3577,10 @@
         <v>7</v>
       </c>
       <c r="B84" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C84" s="7" t="s">
         <v>365</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -3599,10 +3588,10 @@
         <v>7</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3610,10 +3599,10 @@
         <v>7</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3621,10 +3610,10 @@
         <v>7</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3632,10 +3621,10 @@
         <v>7</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3643,10 +3632,10 @@
         <v>7</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3654,10 +3643,10 @@
         <v>7</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3665,10 +3654,10 @@
         <v>7</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3676,10 +3665,10 @@
         <v>7</v>
       </c>
       <c r="B92" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="C92" s="7" t="s">
         <v>375</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3687,10 +3676,10 @@
         <v>7</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3698,10 +3687,10 @@
         <v>7</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3709,10 +3698,10 @@
         <v>7</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3720,10 +3709,10 @@
         <v>7</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3731,10 +3720,10 @@
         <v>7</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -3742,10 +3731,10 @@
         <v>7</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3753,10 +3742,10 @@
         <v>7</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3764,10 +3753,10 @@
         <v>7</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3775,10 +3764,10 @@
         <v>7</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -3786,10 +3775,10 @@
         <v>7</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3797,10 +3786,10 @@
         <v>7</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -3808,10 +3797,10 @@
         <v>8</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -3819,10 +3808,10 @@
         <v>8</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -3830,10 +3819,10 @@
         <v>8</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -3841,10 +3830,10 @@
         <v>8</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -3852,10 +3841,10 @@
         <v>8</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -3863,10 +3852,10 @@
         <v>8</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
@@ -3874,10 +3863,10 @@
         <v>8</v>
       </c>
       <c r="B110" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="C110" s="7" t="s">
         <v>445</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -3885,10 +3874,10 @@
         <v>8</v>
       </c>
       <c r="B111" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C111" s="7" t="s">
         <v>421</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -3896,10 +3885,10 @@
         <v>8</v>
       </c>
       <c r="B112" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -3907,10 +3896,10 @@
         <v>8</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -3918,10 +3907,10 @@
         <v>8</v>
       </c>
       <c r="B114" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="C114" s="5" t="s">
         <v>426</v>
-      </c>
-      <c r="C114" s="5" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -3929,10 +3918,10 @@
         <v>8</v>
       </c>
       <c r="B115" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C115" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="C115" s="5" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -3940,10 +3929,10 @@
         <v>8</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -3951,10 +3940,10 @@
         <v>8</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -3962,10 +3951,10 @@
         <v>8</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -3973,10 +3962,10 @@
         <v>8</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -3984,10 +3973,10 @@
         <v>8</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
@@ -3995,10 +3984,10 @@
         <v>8</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
@@ -4006,10 +3995,10 @@
         <v>8</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
@@ -4017,10 +4006,10 @@
         <v>8</v>
       </c>
       <c r="B123" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C123" s="5" t="s">
         <v>454</v>
-      </c>
-      <c r="C123" s="5" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
@@ -4028,10 +4017,10 @@
         <v>8</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -4039,10 +4028,10 @@
         <v>8</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C125" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4050,10 +4039,10 @@
         <v>8</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -4061,10 +4050,10 @@
         <v>8</v>
       </c>
       <c r="B127" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="C127" s="5" t="s">
         <v>460</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4072,10 +4061,10 @@
         <v>8</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
@@ -4083,10 +4072,10 @@
         <v>8</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
@@ -4094,10 +4083,10 @@
         <v>8</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
@@ -4105,10 +4094,10 @@
         <v>8</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
@@ -4116,10 +4105,10 @@
         <v>8</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -4127,10 +4116,10 @@
         <v>8</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -4138,10 +4127,10 @@
         <v>8</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -4149,10 +4138,10 @@
         <v>8</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -4160,10 +4149,10 @@
         <v>8</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="144" x14ac:dyDescent="0.3">
@@ -4171,10 +4160,10 @@
         <v>8</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="144" x14ac:dyDescent="0.3">
@@ -4182,10 +4171,10 @@
         <v>8</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="144" x14ac:dyDescent="0.3">
@@ -4193,10 +4182,10 @@
         <v>8</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="144" x14ac:dyDescent="0.3">
@@ -4204,10 +4193,10 @@
         <v>8</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -4215,10 +4204,10 @@
         <v>8</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -4226,10 +4215,10 @@
         <v>8</v>
       </c>
       <c r="B142" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="C142" s="5" t="s">
         <v>478</v>
-      </c>
-      <c r="C142" s="5" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -4237,10 +4226,10 @@
         <v>8</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -4248,10 +4237,10 @@
         <v>8</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -4259,10 +4248,10 @@
         <v>8</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -4270,10 +4259,10 @@
         <v>8</v>
       </c>
       <c r="B146" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="C146" s="7" t="s">
         <v>487</v>
-      </c>
-      <c r="C146" s="7" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -4281,10 +4270,10 @@
         <v>8</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4292,10 +4281,10 @@
         <v>8</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4303,10 +4292,10 @@
         <v>8</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4314,10 +4303,10 @@
         <v>8</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4325,10 +4314,10 @@
         <v>8</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4336,10 +4325,10 @@
         <v>8</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4347,10 +4336,10 @@
         <v>8</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4358,10 +4347,10 @@
         <v>8</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4369,10 +4358,10 @@
         <v>8</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -4380,10 +4369,10 @@
         <v>8</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -4391,10 +4380,10 @@
         <v>8</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -4402,10 +4391,10 @@
         <v>8</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
@@ -4413,10 +4402,10 @@
         <v>8</v>
       </c>
       <c r="B159" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="C159" s="5" t="s">
         <v>503</v>
-      </c>
-      <c r="C159" s="5" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
@@ -4424,10 +4413,10 @@
         <v>8</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4435,7 +4424,7 @@
         <v>8</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C161" t="s">
         <v>227</v>
@@ -4446,10 +4435,10 @@
         <v>8</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C162" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4457,10 +4446,10 @@
         <v>8</v>
       </c>
       <c r="B163" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="C163" t="s">
         <v>523</v>
-      </c>
-      <c r="C163" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4468,10 +4457,10 @@
         <v>8</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C164" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -4479,10 +4468,10 @@
         <v>8</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C165" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4490,10 +4479,10 @@
         <v>8</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4501,10 +4490,10 @@
         <v>8</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C167" s="7" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4512,10 +4501,10 @@
         <v>8</v>
       </c>
       <c r="B168" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C168" t="s">
         <v>532</v>
-      </c>
-      <c r="C168" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4523,10 +4512,10 @@
         <v>8</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C169" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -4534,10 +4523,10 @@
         <v>8</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C170" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -4545,10 +4534,10 @@
         <v>8</v>
       </c>
       <c r="B171" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -4556,10 +4545,10 @@
         <v>9</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C172" s="7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4567,10 +4556,10 @@
         <v>9</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C173" s="7" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -4578,10 +4567,10 @@
         <v>9</v>
       </c>
       <c r="B174" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C174" s="5" t="s">
         <v>396</v>
-      </c>
-      <c r="C174" s="5" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
@@ -4589,10 +4578,10 @@
         <v>9</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -4600,10 +4589,10 @@
         <v>9</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C176" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -4611,10 +4600,10 @@
         <v>9</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -4622,10 +4611,10 @@
         <v>9</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4633,10 +4622,10 @@
         <v>9</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4644,10 +4633,10 @@
         <v>9</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C180" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4655,10 +4644,10 @@
         <v>9</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -4666,10 +4655,10 @@
         <v>9</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C182" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -4677,10 +4666,10 @@
         <v>9</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C183" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
@@ -4688,10 +4677,10 @@
         <v>9</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C184" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -4699,10 +4688,10 @@
         <v>9</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C185" s="7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -4710,10 +4699,10 @@
         <v>9</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -4721,10 +4710,10 @@
         <v>9</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4732,10 +4721,10 @@
         <v>9</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4743,10 +4732,10 @@
         <v>9</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -4754,10 +4743,10 @@
         <v>9</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
@@ -4765,10 +4754,10 @@
         <v>9</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -4776,10 +4765,10 @@
         <v>9</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C192" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -4787,10 +4776,10 @@
         <v>9</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C193" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4798,10 +4787,10 @@
         <v>9</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4809,10 +4798,10 @@
         <v>9</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -4820,10 +4809,10 @@
         <v>9</v>
       </c>
       <c r="B196" s="5" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
@@ -4831,10 +4820,10 @@
         <v>9</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4842,10 +4831,10 @@
         <v>9</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4853,10 +4842,10 @@
         <v>9</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C199" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
@@ -4864,10 +4853,10 @@
         <v>9</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4875,10 +4864,10 @@
         <v>9</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4886,10 +4875,10 @@
         <v>9</v>
       </c>
       <c r="B202" s="5" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
@@ -4897,10 +4886,10 @@
         <v>9</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C203" s="5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4908,10 +4897,10 @@
         <v>9</v>
       </c>
       <c r="B204" s="5" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4919,10 +4908,10 @@
         <v>9</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C205" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4930,10 +4919,10 @@
         <v>9</v>
       </c>
       <c r="B206" s="5" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4941,10 +4930,10 @@
         <v>9</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C207" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
@@ -4952,10 +4941,10 @@
         <v>10</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C208" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -4963,10 +4952,10 @@
         <v>10</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
@@ -4974,10 +4963,10 @@
         <v>10</v>
       </c>
       <c r="B210" s="5" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C210" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
@@ -4985,10 +4974,10 @@
         <v>10</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C211" s="5" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
@@ -4996,10 +4985,10 @@
         <v>10</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C212" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -5007,10 +4996,10 @@
         <v>10</v>
       </c>
       <c r="B213" s="5" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C213" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5018,10 +5007,10 @@
         <v>10</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5029,10 +5018,10 @@
         <v>10</v>
       </c>
       <c r="B215" s="5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C215" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -5040,10 +5029,10 @@
         <v>10</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C216" s="5" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
@@ -5051,10 +5040,10 @@
         <v>10</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C217" s="5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5062,10 +5051,10 @@
         <v>10</v>
       </c>
       <c r="B218" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5073,10 +5062,10 @@
         <v>10</v>
       </c>
       <c r="B219" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C219" s="5" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -5084,10 +5073,10 @@
         <v>10</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C220" s="5" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
@@ -5095,10 +5084,10 @@
         <v>10</v>
       </c>
       <c r="B221" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5106,10 +5095,10 @@
         <v>10</v>
       </c>
       <c r="B222" s="5" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C222" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5117,10 +5106,10 @@
         <v>10</v>
       </c>
       <c r="B223" s="5" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C223" s="5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5128,10 +5117,10 @@
         <v>10</v>
       </c>
       <c r="B224" s="5" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C224" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5139,10 +5128,10 @@
         <v>10</v>
       </c>
       <c r="B225" s="5" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C225" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5150,10 +5139,10 @@
         <v>10</v>
       </c>
       <c r="B226" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C226" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5161,10 +5150,10 @@
         <v>10</v>
       </c>
       <c r="B227" s="5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C227" s="5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5172,10 +5161,10 @@
         <v>10</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5183,10 +5172,10 @@
         <v>10</v>
       </c>
       <c r="B229" s="5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -5194,10 +5183,10 @@
         <v>10</v>
       </c>
       <c r="B230" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="C230" s="5" t="s">
         <v>609</v>
-      </c>
-      <c r="C230" s="5" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -5205,10 +5194,10 @@
         <v>10</v>
       </c>
       <c r="B231" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="C231" s="5" t="s">
         <v>610</v>
-      </c>
-      <c r="C231" s="5" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5216,10 +5205,10 @@
         <v>10</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5227,10 +5216,10 @@
         <v>10</v>
       </c>
       <c r="B233" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="C233" s="5" t="s">
         <v>615</v>
-      </c>
-      <c r="C233" s="5" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -5238,10 +5227,10 @@
         <v>10</v>
       </c>
       <c r="B234" s="5" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
@@ -5249,74 +5238,74 @@
         <v>11</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C235" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B236" s="12" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C236" s="12" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B237" s="5" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C237" s="12" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B238" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B239" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C239" s="5" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B240" s="5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C240" s="5" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="241" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B241" s="5" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="242" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B242" s="5" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C242" s="5" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="243" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B243" s="5" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C243" s="5" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -5326,10 +5315,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A0C351-3687-474E-A31D-3B46FA24EFD7}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C72" sqref="B1:C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5456,7 +5445,7 @@
         <v>220</v>
       </c>
       <c r="C11" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -5585,10 +5574,10 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>244</v>
+        <v>673</v>
       </c>
       <c r="C23" t="s">
-        <v>245</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -5596,10 +5585,10 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -5607,10 +5596,10 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C25" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -5618,10 +5607,10 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C26" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -5629,10 +5618,10 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C27" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -5640,10 +5629,10 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C28" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -5651,10 +5640,10 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C29" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -5662,10 +5651,10 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -5673,10 +5662,10 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C31" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -5684,10 +5673,10 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C32" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -5695,10 +5684,10 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C33" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -5706,10 +5695,10 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C34" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -5717,10 +5706,10 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C35" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -5728,10 +5717,10 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C36" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -5739,10 +5728,10 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C37" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -5750,10 +5739,10 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C38" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -5761,10 +5750,10 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C39" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -5772,10 +5761,10 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C40" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -5783,10 +5772,10 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C41" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -5794,10 +5783,10 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C42" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -5805,10 +5794,10 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
+        <v>327</v>
+      </c>
+      <c r="C43" t="s">
         <v>329</v>
-      </c>
-      <c r="C43" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -5816,10 +5805,10 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
+        <v>328</v>
+      </c>
+      <c r="C44" t="s">
         <v>330</v>
-      </c>
-      <c r="C44" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -5827,10 +5816,10 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C45" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -5838,10 +5827,10 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C46" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -5849,10 +5838,10 @@
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C47" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -5860,10 +5849,10 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C48" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -5871,10 +5860,10 @@
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C49" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -5882,10 +5871,10 @@
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C50" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -5893,10 +5882,10 @@
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C51" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -5904,10 +5893,10 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C52" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -5915,10 +5904,10 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C53" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -5926,10 +5915,10 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C54" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -5937,10 +5926,10 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C55" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -5948,10 +5937,10 @@
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C56" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -5959,10 +5948,10 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C57" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -5970,10 +5959,10 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C58" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -5981,10 +5970,10 @@
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C59" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -5992,10 +5981,10 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C60" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -6003,10 +5992,10 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C61" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -6014,10 +6003,10 @@
         <v>13</v>
       </c>
       <c r="B62" t="s">
+        <v>649</v>
+      </c>
+      <c r="C62" t="s">
         <v>651</v>
-      </c>
-      <c r="C62" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -6025,10 +6014,10 @@
         <v>13</v>
       </c>
       <c r="B63" t="s">
+        <v>650</v>
+      </c>
+      <c r="C63" t="s">
         <v>652</v>
-      </c>
-      <c r="C63" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -6036,10 +6025,10 @@
         <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C64" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -6047,10 +6036,10 @@
         <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C65" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -6058,10 +6047,10 @@
         <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C66" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -6069,10 +6058,10 @@
         <v>13</v>
       </c>
       <c r="B67" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C67" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -6080,10 +6069,10 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C68" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -6091,10 +6080,10 @@
         <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C69" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -6102,10 +6091,10 @@
         <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C70" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -6113,10 +6102,10 @@
         <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C71" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -6124,21 +6113,10 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="C72" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>36</v>
-      </c>
-      <c r="B73" t="s">
-        <v>676</v>
-      </c>
-      <c r="C73" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
     </row>
   </sheetData>
@@ -6161,31 +6139,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" t="s">
         <v>283</v>
-      </c>
-      <c r="B3" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
         <v>219</v>
@@ -6193,31 +6171,31 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B8" t="s">
         <v>221</v>
@@ -6225,31 +6203,31 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B10" t="s">
         <v>288</v>
-      </c>
-      <c r="B10" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B12" t="s">
         <v>225</v>
@@ -6257,7 +6235,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B13" t="s">
         <v>227</v>
@@ -6265,7 +6243,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B14" t="s">
         <v>228</v>
@@ -6273,15 +6251,15 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B15" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B16" t="s">
         <v>230</v>
@@ -6289,10 +6267,10 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -6300,7 +6278,7 @@
         <v>233</v>
       </c>
       <c r="B18" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -6340,7 +6318,7 @@
         <v>233</v>
       </c>
       <c r="B23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -6353,26 +6331,26 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B27" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -6380,7 +6358,7 @@
         <v>235</v>
       </c>
       <c r="B28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -6388,7 +6366,7 @@
         <v>235</v>
       </c>
       <c r="B29" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -6396,7 +6374,7 @@
         <v>235</v>
       </c>
       <c r="B30" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -6404,7 +6382,7 @@
         <v>235</v>
       </c>
       <c r="B31" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -6412,7 +6390,7 @@
         <v>236</v>
       </c>
       <c r="B32" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -6420,7 +6398,7 @@
         <v>236</v>
       </c>
       <c r="B33" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -6428,7 +6406,7 @@
         <v>236</v>
       </c>
       <c r="B34" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -6436,7 +6414,7 @@
         <v>236</v>
       </c>
       <c r="B35" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -6444,7 +6422,7 @@
         <v>236</v>
       </c>
       <c r="B36" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -6452,7 +6430,7 @@
         <v>236</v>
       </c>
       <c r="B37" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -6460,7 +6438,7 @@
         <v>238</v>
       </c>
       <c r="B38" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -6468,7 +6446,7 @@
         <v>238</v>
       </c>
       <c r="B39" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -6476,7 +6454,7 @@
         <v>238</v>
       </c>
       <c r="B40" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -6484,263 +6462,263 @@
         <v>238</v>
       </c>
       <c r="B41" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B42" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B43" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B44" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B45" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B46" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B47" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B48" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B49" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B50" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B51" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B52" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B53" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B54" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B55" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="B56" t="s">
         <v>340</v>
-      </c>
-      <c r="B56" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B57" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B58" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B59" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B60" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B61" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B62" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B63" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B64" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B65" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B66" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B67" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B68" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B69" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B70" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B71" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B72" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B73" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -6752,72 +6730,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE37008-7EF0-48F4-B41A-7A9922CF3695}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
+    <sheetView zoomScale="71" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" style="14" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="46.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="B1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>695</v>
+      </c>
+      <c r="B2" t="s">
         <v>692</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C2">
+        <v>513</v>
+      </c>
+      <c r="D2" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>695</v>
+      </c>
+      <c r="B3" t="s">
         <v>693</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="C3">
+        <v>513</v>
+      </c>
+      <c r="D3" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>695</v>
+      </c>
+      <c r="B4" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>698</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>695</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="C4">
         <v>513</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
-        <v>698</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="D4" t="s">
         <v>696</v>
-      </c>
-      <c r="C3" s="14">
-        <v>513</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>698</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>697</v>
-      </c>
-      <c r="C4" s="14">
-        <v>513</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>699</v>
       </c>
     </row>
   </sheetData>
@@ -6976,7 +6953,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -6990,7 +6967,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -7032,7 +7009,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -7088,7 +7065,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -7298,7 +7275,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -7382,7 +7359,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -7396,7 +7373,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -7410,7 +7387,7 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -7522,7 +7499,7 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -7536,7 +7513,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -7550,7 +7527,7 @@
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -7564,7 +7541,7 @@
         <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -7578,7 +7555,7 @@
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -7592,7 +7569,7 @@
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -7606,7 +7583,7 @@
         <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -7704,7 +7681,7 @@
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -7734,7 +7711,7 @@
         <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -7745,7 +7722,7 @@
         <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -7756,7 +7733,7 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -7767,7 +7744,7 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -7778,7 +7755,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -7789,7 +7766,7 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -7800,7 +7777,7 @@
         <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -7811,7 +7788,7 @@
         <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -7822,7 +7799,7 @@
         <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -7833,7 +7810,7 @@
         <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -7841,10 +7818,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>684</v>
+      </c>
+      <c r="C11" t="s">
         <v>687</v>
-      </c>
-      <c r="C11" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -7855,7 +7832,7 @@
         <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -7863,10 +7840,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C13" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>